<commit_message>
feat(products): extend product schema, import logic, and UI for expanded assortment analytics
This update adds support for detailed product analytics and mapping by introducing
new product fields, advanced XLSX/CSV header parsing, and an enhanced editable UI.
- Expanded Product model and migration: added fields for marketplace codes,
  packaging, weight, logistics, pricing components, stock breakdown, and
  custom JSON data for compatibility and extensibility
- Improved import: Russian header mapping, automatic numeric parsing, price
  recomputation, and safe merging of legacy data
- Enhanced UI: editable grid covers core/new fields, metrics like margin,
  commission, and price_final are showcased as read-only, type and format
  validation, JSON viewer for metadata, and better doc/sample files
- README/table schema and templates updated for clarity on all columns

No breaking changes; backward compatibility maintained for legacy Extra fields.
</commit_message>
<xml_diff>
--- a/data/products_import_sample.xlsx
+++ b/data/products_import_sample.xlsx
@@ -14,11 +14,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="53">
   <si>
     <t>sku</t>
   </si>
   <si>
+    <t>seller_sku</t>
+  </si>
+  <si>
+    <t>wb_sku</t>
+  </si>
+  <si>
     <t>nm_id</t>
   </si>
   <si>
@@ -31,91 +37,142 @@
     <t>category</t>
   </si>
   <si>
+    <t>price_src</t>
+  </si>
+  <si>
+    <t>seller_discount_pct</t>
+  </si>
+  <si>
     <t>price</t>
   </si>
   <si>
+    <t>price_final</t>
+  </si>
+  <si>
     <t>stock</t>
   </si>
   <si>
+    <t>stock_wb</t>
+  </si>
+  <si>
+    <t>stock_seller</t>
+  </si>
+  <si>
     <t>barcode</t>
   </si>
   <si>
     <t>is_active</t>
   </si>
   <si>
-    <t>color</t>
-  </si>
-  <si>
-    <t>size</t>
-  </si>
-  <si>
-    <t>season</t>
+    <t>product_cost</t>
+  </si>
+  <si>
+    <t>shipping_cost</t>
+  </si>
+  <si>
+    <t>logistics_back_cost</t>
+  </si>
+  <si>
+    <t>warehouse_coeff</t>
+  </si>
+  <si>
+    <t>turnover_days</t>
+  </si>
+  <si>
+    <t>weight_kg</t>
+  </si>
+  <si>
+    <t>package_l_cm</t>
+  </si>
+  <si>
+    <t>package_w_cm</t>
+  </si>
+  <si>
+    <t>package_h_cm</t>
   </si>
   <si>
     <t>volume_l</t>
   </si>
   <si>
-    <t>WB-20001</t>
-  </si>
-  <si>
-    <t>WB-20002</t>
-  </si>
-  <si>
-    <t>WB-20003</t>
-  </si>
-  <si>
-    <t>Футболка унисекс с принтом</t>
-  </si>
-  <si>
-    <t>Легинсы спортивные</t>
-  </si>
-  <si>
-    <t>Рюкзак городской водоотталкивающий</t>
-  </si>
-  <si>
-    <t>DemoWear</t>
-  </si>
-  <si>
-    <t>Urban Demo</t>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>custom_data</t>
+  </si>
+  <si>
+    <t>WB-10001</t>
+  </si>
+  <si>
+    <t>WB-10002</t>
+  </si>
+  <si>
+    <t>WB-10003</t>
+  </si>
+  <si>
+    <t>SELLER-10001</t>
+  </si>
+  <si>
+    <t>SELLER-10002</t>
+  </si>
+  <si>
+    <t>SELLER-10003</t>
+  </si>
+  <si>
+    <t>WB-10001-01</t>
+  </si>
+  <si>
+    <t>WB-10002-01</t>
+  </si>
+  <si>
+    <t>WB-10003-01</t>
+  </si>
+  <si>
+    <t>Футболка мужская базовая</t>
+  </si>
+  <si>
+    <t>Худи оверсайз женское</t>
+  </si>
+  <si>
+    <t>Рюкзак городской</t>
+  </si>
+  <si>
+    <t>MockWear</t>
+  </si>
+  <si>
+    <t>Urban Mock</t>
   </si>
   <si>
     <t>Одежда</t>
   </si>
   <si>
-    <t>Спорт</t>
-  </si>
-  <si>
     <t>Аксессуары</t>
   </si>
   <si>
-    <t>9900011122234</t>
-  </si>
-  <si>
-    <t>9900011122235</t>
-  </si>
-  <si>
-    <t>9900011122236</t>
-  </si>
-  <si>
-    <t>Белый</t>
-  </si>
-  <si>
-    <t>Черный</t>
-  </si>
-  <si>
-    <t>Серый</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>SS24</t>
-  </si>
-  <si>
-    <t>AW24</t>
+    <t>1112223334445</t>
+  </si>
+  <si>
+    <t>1112223334446</t>
+  </si>
+  <si>
+    <t>1112223334447</t>
+  </si>
+  <si>
+    <t>Базовая позиция</t>
+  </si>
+  <si>
+    <t>Сезонная коллекция</t>
+  </si>
+  <si>
+    <t>Влагостойкий материал</t>
+  </si>
+  <si>
+    <t>{"commission_pct": 15, "tax_pct": 6}</t>
+  </si>
+  <si>
+    <t>{"commission_pct": 18, "tax_pct": 6}</t>
+  </si>
+  <si>
+    <t>{"commission_pct": 17, "tax_pct": 6}</t>
   </si>
 </sst>
 </file>
@@ -473,13 +530,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:AB4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:28">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -519,116 +576,308 @@
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:28">
       <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2">
-        <v>20001</v>
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
-        <v>19</v>
+        <v>34</v>
+      </c>
+      <c r="D2">
+        <v>10001</v>
       </c>
       <c r="E2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2">
+        <v>1299</v>
+      </c>
+      <c r="I2">
+        <v>10</v>
+      </c>
+      <c r="J2">
+        <v>1169.1</v>
+      </c>
+      <c r="K2">
+        <v>1169.1</v>
+      </c>
+      <c r="L2">
+        <v>45</v>
+      </c>
+      <c r="M2">
+        <v>30</v>
+      </c>
+      <c r="N2">
+        <v>15</v>
+      </c>
+      <c r="O2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P2" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>620</v>
+      </c>
+      <c r="R2">
+        <v>45</v>
+      </c>
+      <c r="S2">
+        <v>20</v>
+      </c>
+      <c r="T2">
+        <v>35</v>
+      </c>
+      <c r="U2">
+        <v>12</v>
+      </c>
+      <c r="V2">
+        <v>0.35</v>
+      </c>
+      <c r="W2">
+        <v>34</v>
+      </c>
+      <c r="X2">
+        <v>24</v>
+      </c>
+      <c r="Y2">
+        <v>4</v>
+      </c>
+      <c r="Z2">
+        <v>3.264</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3">
+        <v>10002</v>
+      </c>
+      <c r="E3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3">
+        <v>2499</v>
+      </c>
+      <c r="I3">
+        <v>15</v>
+      </c>
+      <c r="J3">
+        <v>2124.15</v>
+      </c>
+      <c r="K3">
+        <v>2124.15</v>
+      </c>
+      <c r="L3">
+        <v>30</v>
+      </c>
+      <c r="M3">
+        <v>18</v>
+      </c>
+      <c r="N3">
+        <v>12</v>
+      </c>
+      <c r="O3" t="s">
+        <v>45</v>
+      </c>
+      <c r="P3" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>980</v>
+      </c>
+      <c r="R3">
+        <v>65</v>
+      </c>
+      <c r="S3">
+        <v>28</v>
+      </c>
+      <c r="T3">
+        <v>42</v>
+      </c>
+      <c r="U3">
+        <v>18</v>
+      </c>
+      <c r="V3">
+        <v>0.58</v>
+      </c>
+      <c r="W3">
+        <v>40</v>
+      </c>
+      <c r="X3">
+        <v>28</v>
+      </c>
+      <c r="Y3">
+        <v>8</v>
+      </c>
+      <c r="Z3">
+        <v>8.960000000000001</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4">
+        <v>10003</v>
+      </c>
+      <c r="E4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4">
+        <v>1899</v>
+      </c>
+      <c r="I4">
+        <v>12</v>
+      </c>
+      <c r="J4">
+        <v>1671.12</v>
+      </c>
+      <c r="K4">
+        <v>1671.12</v>
+      </c>
+      <c r="L4">
+        <v>18</v>
+      </c>
+      <c r="M4">
+        <v>10</v>
+      </c>
+      <c r="N4">
+        <v>8</v>
+      </c>
+      <c r="O4" t="s">
+        <v>46</v>
+      </c>
+      <c r="P4" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <v>780</v>
+      </c>
+      <c r="R4">
+        <v>55</v>
+      </c>
+      <c r="S4">
+        <v>25</v>
+      </c>
+      <c r="T4">
+        <v>38</v>
+      </c>
+      <c r="U4">
         <v>21</v>
       </c>
-      <c r="F2">
-        <v>1499</v>
-      </c>
-      <c r="G2">
-        <v>60</v>
-      </c>
-      <c r="H2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J2" t="s">
-        <v>27</v>
-      </c>
-      <c r="K2" t="s">
-        <v>30</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="V4">
+        <v>0.74</v>
+      </c>
+      <c r="W4">
+        <v>45</v>
+      </c>
+      <c r="X4">
         <v>32</v>
       </c>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3">
-        <v>20002</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3">
-        <v>1799</v>
-      </c>
-      <c r="G3">
-        <v>35</v>
-      </c>
-      <c r="H3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J3" t="s">
-        <v>28</v>
-      </c>
-      <c r="K3" t="s">
-        <v>31</v>
-      </c>
-      <c r="L3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4">
-        <v>20003</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4">
-        <v>2199</v>
-      </c>
-      <c r="G4">
-        <v>22</v>
-      </c>
-      <c r="H4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" t="b">
-        <v>1</v>
-      </c>
-      <c r="J4" t="s">
-        <v>29</v>
-      </c>
-      <c r="M4">
-        <v>20</v>
+      <c r="Y4">
+        <v>12</v>
+      </c>
+      <c r="Z4">
+        <v>17.28</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(products/import): improve field mapping, UI labels, and documentation for product schema
Enhance import mapping and field normalization for provided Russian column headers.
Update sample templates, computed columns, and product UI with localized
labels and improved field suggestions. Rewrite README with up-to-date table of
catalog columns and template usage. Columns like 'литраж/Литраж' are unified,
additional aliases for dimensions and boolean fields ('Активен') are mapped,
and computed/read-only fields have clearer UI hints.

This change increases reliability and clarity in import/export flows, makes UX
friendlier for native users, and ensures that documentation and templates
accurately reflect schema and UI expectations. No breaking changes for existing
API users, but old import templates should be regenerated to match new labels.
</commit_message>
<xml_diff>
--- a/data/products_import_sample.xlsx
+++ b/data/products_import_sample.xlsx
@@ -14,90 +14,90 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="53">
-  <si>
-    <t>sku</t>
-  </si>
-  <si>
-    <t>seller_sku</t>
-  </si>
-  <si>
-    <t>wb_sku</t>
-  </si>
-  <si>
-    <t>nm_id</t>
-  </si>
-  <si>
-    <t>title</t>
-  </si>
-  <si>
-    <t>brand</t>
-  </si>
-  <si>
-    <t>category</t>
-  </si>
-  <si>
-    <t>price_src</t>
-  </si>
-  <si>
-    <t>seller_discount_pct</t>
-  </si>
-  <si>
-    <t>price</t>
-  </si>
-  <si>
-    <t>price_final</t>
-  </si>
-  <si>
-    <t>stock</t>
-  </si>
-  <si>
-    <t>stock_wb</t>
-  </si>
-  <si>
-    <t>stock_seller</t>
-  </si>
-  <si>
-    <t>barcode</t>
-  </si>
-  <si>
-    <t>is_active</t>
-  </si>
-  <si>
-    <t>product_cost</t>
-  </si>
-  <si>
-    <t>shipping_cost</t>
-  </si>
-  <si>
-    <t>logistics_back_cost</t>
-  </si>
-  <si>
-    <t>warehouse_coeff</t>
-  </si>
-  <si>
-    <t>turnover_days</t>
-  </si>
-  <si>
-    <t>weight_kg</t>
-  </si>
-  <si>
-    <t>package_l_cm</t>
-  </si>
-  <si>
-    <t>package_w_cm</t>
-  </si>
-  <si>
-    <t>package_h_cm</t>
-  </si>
-  <si>
-    <t>volume_l</t>
-  </si>
-  <si>
-    <t>comments</t>
-  </si>
-  <si>
-    <t>custom_data</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
+  <si>
+    <t>SKU</t>
+  </si>
+  <si>
+    <t>Артикул продавца</t>
+  </si>
+  <si>
+    <t>Артикул WB</t>
+  </si>
+  <si>
+    <t>NM ID</t>
+  </si>
+  <si>
+    <t>Название</t>
+  </si>
+  <si>
+    <t>Бренд</t>
+  </si>
+  <si>
+    <t>Категория</t>
+  </si>
+  <si>
+    <t>Текущая цена</t>
+  </si>
+  <si>
+    <t>Скидка, %</t>
+  </si>
+  <si>
+    <t>Итоговая цена (расчёт)</t>
+  </si>
+  <si>
+    <t>Цена со скидкой (расчёт)</t>
+  </si>
+  <si>
+    <t>Остаток общий (расчёт)</t>
+  </si>
+  <si>
+    <t>Остатки WB</t>
+  </si>
+  <si>
+    <t>Остатки продавца</t>
+  </si>
+  <si>
+    <t>Штрихкод</t>
+  </si>
+  <si>
+    <t>Активен</t>
+  </si>
+  <si>
+    <t>Себик</t>
+  </si>
+  <si>
+    <t>Транспортировка</t>
+  </si>
+  <si>
+    <t>Логистика возврата</t>
+  </si>
+  <si>
+    <t>Коэфф. склада</t>
+  </si>
+  <si>
+    <t>Оборачиваемость, дни</t>
+  </si>
+  <si>
+    <t>Вес с упаковкой (кг)</t>
+  </si>
+  <si>
+    <t>Длина упаковки, см</t>
+  </si>
+  <si>
+    <t>Ширина упаковки, см</t>
+  </si>
+  <si>
+    <t>Высота упаковки, см</t>
+  </si>
+  <si>
+    <t>Литраж</t>
+  </si>
+  <si>
+    <t>Комменты</t>
+  </si>
+  <si>
+    <t>Доп данные JSON</t>
   </si>
   <si>
     <t>WB-10001</t>
@@ -146,15 +146,6 @@
   </si>
   <si>
     <t>Аксессуары</t>
-  </si>
-  <si>
-    <t>1112223334445</t>
-  </si>
-  <si>
-    <t>1112223334446</t>
-  </si>
-  <si>
-    <t>1112223334447</t>
   </si>
   <si>
     <t>Базовая позиция</t>
@@ -665,8 +656,8 @@
       <c r="N2">
         <v>15</v>
       </c>
-      <c r="O2" t="s">
-        <v>44</v>
+      <c r="O2">
+        <v>1112223334445</v>
       </c>
       <c r="P2" t="b">
         <v>1</v>
@@ -702,10 +693,10 @@
         <v>3.264</v>
       </c>
       <c r="AA2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB2" t="s">
         <v>47</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:28">
@@ -751,8 +742,8 @@
       <c r="N3">
         <v>12</v>
       </c>
-      <c r="O3" t="s">
-        <v>45</v>
+      <c r="O3">
+        <v>1112223334446</v>
       </c>
       <c r="P3" t="b">
         <v>1</v>
@@ -788,10 +779,10 @@
         <v>8.960000000000001</v>
       </c>
       <c r="AA3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB3" t="s">
         <v>48</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:28">
@@ -837,8 +828,8 @@
       <c r="N4">
         <v>8</v>
       </c>
-      <c r="O4" t="s">
-        <v>46</v>
+      <c r="O4">
+        <v>1112223334447</v>
       </c>
       <c r="P4" t="b">
         <v>1</v>
@@ -874,10 +865,10 @@
         <v>17.28</v>
       </c>
       <c r="AA4" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB4" t="s">
         <v>49</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>